<commit_message>
dimensionless numbers van Morgan
</commit_message>
<xml_diff>
--- a/other_side_stuff/calculatingdimensionlessnumbers.xlsx
+++ b/other_side_stuff/calculatingdimensionlessnumbers.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sikke\Documents\GitHub\cough-machine-control\other_side_stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31CB0694-1D34-4B85-9ACF-B6D21DF34634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAD762D-F78C-4242-8011-919D3422B8A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9B6FACEC-0DD2-4E04-99F0-4736BE1EF523}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{9B6FACEC-0DD2-4E04-99F0-4736BE1EF523}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Airflow (m/s)</t>
   </si>
@@ -111,15 +112,19 @@
   </si>
   <si>
     <t>Zero shear viscosity (Pa s)</t>
+  </si>
+  <si>
+    <t>Morgan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="0.0000"/>
-    <numFmt numFmtId="175" formatCode="0.0E+00"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0E+00"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -180,18 +185,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -529,7 +535,7 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12:L19"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,6 +548,7 @@
     <col min="8" max="8" width="25.77734375" customWidth="1"/>
     <col min="9" max="9" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="24" customWidth="1"/>
   </cols>
@@ -672,11 +679,11 @@
         <v>44272.844272844268</v>
       </c>
       <c r="K3" s="8">
-        <f>I3*D3/($R$1/1000)</f>
+        <f t="shared" ref="K2:K18" si="2">I3*D3/($R$1/1000)</f>
         <v>95</v>
       </c>
       <c r="L3" s="8">
-        <f t="shared" ref="L3:L10" si="2">$R$6*D3^2 * (F3/1000)/ ($R$3)</f>
+        <f t="shared" ref="L3:L10" si="3">$R$6*D3^2 * (F3/1000)/ ($R$3)</f>
         <v>40.802125506072876</v>
       </c>
       <c r="Q3" t="s">
@@ -720,11 +727,11 @@
         <v>44272.844272844268</v>
       </c>
       <c r="K4" s="8">
-        <f>I4*D4/($R$1/1000)</f>
+        <f t="shared" si="2"/>
         <v>25.5</v>
       </c>
       <c r="L4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40.802125506072876</v>
       </c>
       <c r="Q4" t="s">
@@ -768,11 +775,11 @@
         <v>44272.844272844268</v>
       </c>
       <c r="K5" s="8">
-        <f>I5*D5/($R$1/1000)</f>
+        <f t="shared" si="2"/>
         <v>3.1</v>
       </c>
       <c r="L5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27.201417004048579</v>
       </c>
       <c r="Q5" t="s">
@@ -816,11 +823,11 @@
         <v>44272.844272844268</v>
       </c>
       <c r="K6" s="8">
-        <f>I6*D6/($R$1/1000)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27.201417004048579</v>
       </c>
       <c r="Q6" t="s">
@@ -864,11 +871,11 @@
         <v>35418.275418275414</v>
       </c>
       <c r="K7" s="8">
-        <f>I7*D7/($R$1/1000)</f>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="L7" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26.113360323886639</v>
       </c>
     </row>
@@ -906,11 +913,11 @@
         <v>39845.559845559837</v>
       </c>
       <c r="K8" s="8">
-        <f>I8*D8/($R$1/1000)</f>
+        <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33.04972165991903</v>
       </c>
     </row>
@@ -948,11 +955,11 @@
         <v>44272.844272844268</v>
       </c>
       <c r="K9" s="8">
-        <f>I9*D9/($R$1/1000)</f>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="L9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27.201417004048579</v>
       </c>
       <c r="Q9" t="s">
@@ -997,11 +1004,11 @@
         <v>44272.844272844268</v>
       </c>
       <c r="K10" s="8">
-        <f>I10*D10/($R$1/1000)</f>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="L10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27.201417004048579</v>
       </c>
       <c r="Q10" t="s">
@@ -1012,49 +1019,113 @@
         <v>1520</v>
       </c>
     </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K11" s="8"/>
+    </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="I12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="8"/>
       <c r="L12" s="10"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="I13" s="10"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="8"/>
       <c r="L13" s="10"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="I14" s="10"/>
-      <c r="K14" s="10"/>
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>44</v>
+      </c>
+      <c r="G14">
+        <v>0.05</v>
+      </c>
+      <c r="I14" s="11">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="K14" s="8">
+        <f>I14*D14/($R$1/1000)</f>
+        <v>1.1439999999999999</v>
+      </c>
       <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="I15" s="10"/>
-      <c r="K15" s="10"/>
+      <c r="D15">
+        <v>44</v>
+      </c>
+      <c r="G15">
+        <v>0.1</v>
+      </c>
+      <c r="I15" s="10">
+        <v>4.0999999999999999E-4</v>
+      </c>
+      <c r="K15" s="8">
+        <f t="shared" si="2"/>
+        <v>1.804</v>
+      </c>
       <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="I16" s="10"/>
-      <c r="K16" s="10"/>
+      <c r="D16">
+        <v>44</v>
+      </c>
+      <c r="G16">
+        <v>0.2</v>
+      </c>
+      <c r="I16" s="10">
+        <v>6.2E-4</v>
+      </c>
+      <c r="K16" s="8">
+        <f t="shared" si="2"/>
+        <v>2.7279999999999998</v>
+      </c>
       <c r="L16" s="10"/>
     </row>
-    <row r="17" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="I17" s="10"/>
-      <c r="K17" s="10"/>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>44</v>
+      </c>
+      <c r="G17">
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="10">
+        <v>1.3600000000000001E-3</v>
+      </c>
+      <c r="K17" s="8">
+        <f t="shared" si="2"/>
+        <v>5.984</v>
+      </c>
       <c r="L17" s="10"/>
     </row>
-    <row r="18" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="I18" s="10"/>
-      <c r="K18" s="10"/>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>44</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="I18" s="10">
+        <v>2.5799999999999998E-3</v>
+      </c>
+      <c r="K18" s="8">
+        <f t="shared" si="2"/>
+        <v>11.351999999999999</v>
+      </c>
       <c r="L18" s="10"/>
     </row>
-    <row r="19" spans="9:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:12" x14ac:dyDescent="0.3">
       <c r="I19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
     </row>
-    <row r="20" spans="9:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:12" x14ac:dyDescent="0.3">
       <c r="I20" s="10">
-        <f t="shared" ref="I13:I23" si="3">I10*1000</f>
+        <f t="shared" ref="I20" si="4">I10*1000</f>
         <v>19</v>
       </c>
       <c r="K20" s="10">
@@ -1064,19 +1135,31 @@
         <v>27.201417004048579</v>
       </c>
     </row>
-    <row r="21" spans="9:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="9:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="9:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="9:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
       <c r="I24" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB81D4C-D6A3-4420-8663-C326AE47DCEC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Just a lof of small changes
</commit_message>
<xml_diff>
--- a/other_side_stuff/calculatingdimensionlessnumbers.xlsx
+++ b/other_side_stuff/calculatingdimensionlessnumbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sikke\Documents\GitHub\cough-machine-control\other_side_stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAD762D-F78C-4242-8011-919D3422B8A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB785CF6-62D9-427B-9832-E3B249217673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{9B6FACEC-0DD2-4E04-99F0-4736BE1EF523}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9B6FACEC-0DD2-4E04-99F0-4736BE1EF523}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -121,10 +121,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
-    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -185,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -197,7 +198,8 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -535,7 +537,7 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,8 +550,7 @@
     <col min="8" max="8" width="25.77734375" customWidth="1"/>
     <col min="9" max="9" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="24" customWidth="1"/>
   </cols>
   <sheetData>
@@ -679,7 +680,7 @@
         <v>44272.844272844268</v>
       </c>
       <c r="K3" s="8">
-        <f t="shared" ref="K2:K18" si="2">I3*D3/($R$1/1000)</f>
+        <f t="shared" ref="K3:K18" si="2">I3*D3/($R$1/1000)</f>
         <v>95</v>
       </c>
       <c r="L3" s="8">
@@ -774,8 +775,8 @@
         <f t="shared" si="1"/>
         <v>44272.844272844268</v>
       </c>
-      <c r="K5" s="8">
-        <f t="shared" si="2"/>
+      <c r="K5" s="12">
+        <f>I5*D5/($R$1/1000)</f>
         <v>3.1</v>
       </c>
       <c r="L5" s="8">
@@ -1077,7 +1078,7 @@
       <c r="G16">
         <v>0.2</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="11">
         <v>6.2E-4</v>
       </c>
       <c r="K16" s="8">

</xml_diff>